<commit_message>
add loan card creation
</commit_message>
<xml_diff>
--- a/public/res/ClothingDemands-RAFBoulmer.xlsx
+++ b/public/res/ClothingDemands-RAFBoulmer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\My Documents\Cadets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\RASPBERRYPI\share\sqnWebsite\public\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B380FAD8-B5FA-4FE3-ABD3-2CD9CE0CC20A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B863B968-FF84-40FF-A88D-BC8A5F16EF3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -1025,9 +1025,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1037,6 +1037,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1285,7 +1286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1343,9 +1344,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1372,43 +1370,51 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="174" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="174" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1417,6 +1423,15 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1430,40 +1445,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1802,11 +1804,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:I56"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1845,29 +1847,29 @@
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
       <c r="J6" s="6"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
@@ -1894,12 +1896,12 @@
       <c r="A8" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:14" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1931,7 +1933,7 @@
       <c r="B13" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="52" t="s">
         <v>100</v>
       </c>
       <c r="D13" s="43"/>
@@ -2035,18 +2037,18 @@
       <c r="A25" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="B25" s="36"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
       <c r="G25" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" s="9" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2061,17 +2063,17 @@
       <c r="I26" s="15"/>
     </row>
     <row r="28" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="48"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47"/>
     </row>
     <row r="29" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
@@ -2079,43 +2081,43 @@
       <c r="C29" s="17"/>
     </row>
     <row r="30" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
     </row>
     <row r="33" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -2124,9 +2126,9 @@
       <c r="F34" s="18" t="s">
         <v>305</v>
       </c>
-      <c r="G34" s="52"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
       <c r="J34" s="9"/>
     </row>
     <row r="35" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2142,12 +2144,12 @@
       <c r="F36" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="G36" s="52">
+      <c r="G36" s="44">
         <f>D25</f>
         <v>0</v>
       </c>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
     </row>
     <row r="37" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11"/>
@@ -2161,9 +2163,9 @@
       <c r="F38" s="18" t="s">
         <v>307</v>
       </c>
-      <c r="G38" s="52"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
       <c r="J38" s="9"/>
     </row>
     <row r="39" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2176,23 +2178,23 @@
       <c r="F40" s="18" t="s">
         <v>308</v>
       </c>
-      <c r="G40" s="55"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="56"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="49"/>
       <c r="J40" s="9"/>
     </row>
     <row r="41" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="50"/>
-      <c r="I41" s="50"/>
+      <c r="B41" s="51"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="51"/>
     </row>
     <row r="42" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
@@ -2200,43 +2202,43 @@
       <c r="C42" s="9"/>
     </row>
     <row r="43" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="B43" s="45"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="45"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="40"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
     </row>
     <row r="44" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="46" t="s">
+      <c r="A44" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
     </row>
     <row r="45" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="44" t="s">
+      <c r="A45" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
     </row>
     <row r="46" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
@@ -2247,30 +2249,30 @@
       <c r="F46" s="22"/>
     </row>
     <row r="47" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="s">
+      <c r="A47" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="45"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="40"/>
+      <c r="H47" s="40"/>
+      <c r="I47" s="40"/>
     </row>
     <row r="48" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="44" t="s">
+      <c r="A48" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="45"/>
-      <c r="I48" s="45"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="40"/>
     </row>
     <row r="49" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
@@ -2281,125 +2283,120 @@
       <c r="F49" s="22"/>
     </row>
     <row r="50" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="44" t="s">
+      <c r="A50" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="45"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
+      <c r="H50" s="40"/>
+      <c r="I50" s="40"/>
     </row>
     <row r="51" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="46" t="s">
+      <c r="A51" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="45"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
-      <c r="G51" s="45"/>
-      <c r="H51" s="45"/>
-      <c r="I51" s="45"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="40"/>
     </row>
     <row r="52" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="44" t="s">
+      <c r="A52" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="B52" s="45"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45"/>
-      <c r="F52" s="45"/>
-      <c r="G52" s="45"/>
-      <c r="H52" s="45"/>
-      <c r="I52" s="45"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="40"/>
+      <c r="H52" s="40"/>
+      <c r="I52" s="40"/>
     </row>
     <row r="54" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="44" t="s">
+      <c r="A54" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="B54" s="45"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="45"/>
-      <c r="F54" s="45"/>
-      <c r="G54" s="45"/>
-      <c r="H54" s="45"/>
-      <c r="I54" s="45"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="40"/>
     </row>
     <row r="55" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="46" t="s">
+      <c r="A55" s="41" t="s">
         <v>309</v>
       </c>
-      <c r="B55" s="45"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="45"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="40"/>
     </row>
     <row r="56" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="46" t="s">
+      <c r="A56" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="B56" s="45"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="45"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="40"/>
     </row>
     <row r="58" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="57" t="s">
+      <c r="A58" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="B58" s="58"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="58"/>
-      <c r="E58" s="58"/>
-      <c r="F58" s="58"/>
-      <c r="G58" s="58"/>
-      <c r="H58" s="58"/>
-      <c r="I58" s="58"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="38"/>
+      <c r="F58" s="38"/>
+      <c r="G58" s="38"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
     </row>
     <row r="59" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="57" t="s">
+      <c r="A59" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="B59" s="58"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="58"/>
-      <c r="F59" s="58"/>
-      <c r="G59" s="58"/>
-      <c r="H59" s="58"/>
-      <c r="I59" s="58"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="38"/>
+      <c r="G59" s="38"/>
+      <c r="H59" s="38"/>
+      <c r="I59" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="A59:I59"/>
-    <mergeCell ref="A48:I48"/>
-    <mergeCell ref="A47:I47"/>
-    <mergeCell ref="A45:I45"/>
-    <mergeCell ref="A44:I44"/>
-    <mergeCell ref="A58:I58"/>
-    <mergeCell ref="A56:I56"/>
-    <mergeCell ref="A55:I55"/>
-    <mergeCell ref="A54:I54"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="A28:I28"/>
+  <mergeCells count="34">
+    <mergeCell ref="A5:I6"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="A52:I52"/>
+    <mergeCell ref="A51:I51"/>
+    <mergeCell ref="A50:I50"/>
+    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="A43:I43"/>
     <mergeCell ref="G40:I40"/>
     <mergeCell ref="A41:I41"/>
     <mergeCell ref="C13:G13"/>
@@ -2411,79 +2408,83 @@
     <mergeCell ref="G38:I38"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="A5:I6"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="A52:I52"/>
-    <mergeCell ref="A51:I51"/>
-    <mergeCell ref="A50:I50"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="A43:I43"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A59:I59"/>
+    <mergeCell ref="A48:I48"/>
+    <mergeCell ref="A47:I47"/>
+    <mergeCell ref="A45:I45"/>
+    <mergeCell ref="A44:I44"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="A56:I56"/>
+    <mergeCell ref="A55:I55"/>
+    <mergeCell ref="A54:I54"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="77" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="75" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="35" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" style="35" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="35" customWidth="1"/>
-    <col min="5" max="5" width="1" style="35" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="35" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" style="35" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="35" customWidth="1"/>
-    <col min="10" max="10" width="1" style="35" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="35" customWidth="1"/>
-    <col min="13" max="13" width="5.85546875" style="35" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="1" style="35" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="35" customWidth="1"/>
-    <col min="18" max="18" width="5.85546875" style="35" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" style="35" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="35"/>
+    <col min="1" max="1" width="18.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="34" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="34" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="34" customWidth="1"/>
+    <col min="5" max="5" width="1" style="34" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="34" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="34" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="34" customWidth="1"/>
+    <col min="10" max="10" width="1" style="34" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="34" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" style="34" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="1" style="34" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" style="34" customWidth="1"/>
+    <col min="18" max="18" width="5.85546875" style="34" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="24" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="62" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
     </row>
     <row r="2" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K2" s="25"/>
@@ -2492,1487 +2493,1488 @@
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="75">
         <f>'Cover Sheet'!B25</f>
         <v>0</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="74">
-        <f>'Cover Sheet'!B8:G8</f>
+      <c r="E3" s="28"/>
+      <c r="F3" s="72">
+        <f>'Cover Sheet'!B8</f>
         <v>0</v>
       </c>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="76"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="74"/>
       <c r="K3" s="25"/>
     </row>
     <row r="4" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="61" t="s">
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="65" t="s">
         <v>162</v>
       </c>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="69" t="s">
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="58" t="s">
         <v>200</v>
       </c>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="69" t="s">
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="Q4" s="70"/>
-      <c r="R4" s="70"/>
-      <c r="S4" s="70"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
     </row>
     <row r="5" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="31" t="s">
+      <c r="E5" s="31"/>
+      <c r="F5" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="J5" s="32"/>
-      <c r="K5" s="33" t="s">
+      <c r="J5" s="31"/>
+      <c r="K5" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="L5" s="31" t="s">
+      <c r="L5" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="N5" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="O5" s="32"/>
-      <c r="P5" s="31" t="s">
+      <c r="O5" s="31"/>
+      <c r="P5" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="Q5" s="31" t="s">
+      <c r="Q5" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="R5" s="31" t="s">
+      <c r="R5" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="S5" s="31" t="s">
+      <c r="S5" s="30" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="31" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="33" t="s">
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="31" t="s">
+      <c r="L6" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="31" t="s">
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="Q6" s="31" t="s">
+      <c r="Q6" s="30" t="s">
         <v>268</v>
       </c>
-      <c r="R6" s="31"/>
-      <c r="S6" s="31"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
     </row>
     <row r="7" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="31" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="33" t="s">
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="L7" s="31" t="s">
+      <c r="L7" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="31" t="s">
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="Q7" s="31" t="s">
+      <c r="Q7" s="30" t="s">
         <v>269</v>
       </c>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30"/>
     </row>
     <row r="8" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="31" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="33" t="s">
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="L8" s="31" t="s">
+      <c r="L8" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="31" t="s">
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="Q8" s="31" t="s">
+      <c r="Q8" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="30"/>
     </row>
     <row r="9" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="31" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="33" t="s">
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="30" t="s">
         <v>204</v>
       </c>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="31" t="s">
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="Q9" s="31" t="s">
+      <c r="Q9" s="30" t="s">
         <v>271</v>
       </c>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
     </row>
     <row r="10" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="31" t="s">
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="33" t="s">
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="L10" s="31" t="s">
+      <c r="L10" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="31" t="s">
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="Q10" s="31" t="s">
+      <c r="Q10" s="30" t="s">
         <v>272</v>
       </c>
-      <c r="R10" s="31"/>
-      <c r="S10" s="31"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
     </row>
     <row r="11" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="31" t="s">
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="33" t="s">
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="L11" s="31" t="s">
+      <c r="L11" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="31" t="s">
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="Q11" s="31" t="s">
+      <c r="Q11" s="30" t="s">
         <v>273</v>
       </c>
-      <c r="R11" s="31"/>
-      <c r="S11" s="31"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
     </row>
     <row r="12" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="31" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="33" t="s">
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="L12" s="31" t="s">
+      <c r="L12" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="31" t="s">
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="30" t="s">
         <v>249</v>
       </c>
-      <c r="Q12" s="31" t="s">
+      <c r="Q12" s="30" t="s">
         <v>274</v>
       </c>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
     </row>
     <row r="13" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="31" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="33" t="s">
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="L13" s="31" t="s">
+      <c r="L13" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="31" t="s">
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="30" t="s">
         <v>250</v>
       </c>
-      <c r="Q13" s="31" t="s">
+      <c r="Q13" s="30" t="s">
         <v>275</v>
       </c>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
     </row>
     <row r="14" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="31" t="s">
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="33" t="s">
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="L14" s="31" t="s">
+      <c r="L14" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="31" t="s">
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="Q14" s="31" t="s">
+      <c r="Q14" s="30" t="s">
         <v>276</v>
       </c>
-      <c r="R14" s="31"/>
-      <c r="S14" s="31"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
     </row>
     <row r="15" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="31" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="33" t="s">
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="L15" s="31" t="s">
+      <c r="L15" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="31" t="s">
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="Q15" s="31" t="s">
+      <c r="Q15" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="R15" s="31"/>
-      <c r="S15" s="31"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
     </row>
     <row r="16" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="31" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="33" t="s">
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="L16" s="31" t="s">
+      <c r="L16" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="31" t="s">
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="Q16" s="31" t="s">
+      <c r="Q16" s="30" t="s">
         <v>278</v>
       </c>
-      <c r="R16" s="31"/>
-      <c r="S16" s="31"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
     </row>
     <row r="17" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="31" t="s">
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="33" t="s">
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="L17" s="31" t="s">
+      <c r="L17" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="31" t="s">
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="Q17" s="31" t="s">
+      <c r="Q17" s="30" t="s">
         <v>279</v>
       </c>
-      <c r="R17" s="31"/>
-      <c r="S17" s="31"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
     </row>
     <row r="18" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="31" t="s">
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="69" t="s">
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="58" t="s">
         <v>213</v>
       </c>
-      <c r="L18" s="70"/>
-      <c r="M18" s="70"/>
-      <c r="N18" s="70"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="31" t="s">
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="30" t="s">
         <v>255</v>
       </c>
-      <c r="Q18" s="31" t="s">
+      <c r="Q18" s="30" t="s">
         <v>280</v>
       </c>
-      <c r="R18" s="31"/>
-      <c r="S18" s="31"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
     </row>
     <row r="19" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="31" t="s">
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="31" t="s">
+      <c r="G19" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="31" t="s">
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="L19" s="31" t="s">
+      <c r="L19" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="M19" s="31" t="s">
+      <c r="M19" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="N19" s="31" t="s">
+      <c r="N19" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="O19" s="32"/>
-      <c r="P19" s="31" t="s">
+      <c r="O19" s="31"/>
+      <c r="P19" s="30" t="s">
         <v>256</v>
       </c>
-      <c r="Q19" s="31" t="s">
+      <c r="Q19" s="30" t="s">
         <v>281</v>
       </c>
-      <c r="R19" s="31"/>
-      <c r="S19" s="31"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="30"/>
     </row>
     <row r="20" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="31" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="33" t="s">
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="L20" s="31" t="s">
+      <c r="L20" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="31" t="s">
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="30" t="s">
         <v>257</v>
       </c>
-      <c r="Q20" s="31" t="s">
+      <c r="Q20" s="30" t="s">
         <v>282</v>
       </c>
-      <c r="R20" s="31"/>
-      <c r="S20" s="31"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
     </row>
     <row r="21" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="31" t="s">
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="33" t="s">
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="L21" s="31" t="s">
+      <c r="L21" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="31" t="s">
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="30" t="s">
         <v>258</v>
       </c>
-      <c r="Q21" s="31" t="s">
+      <c r="Q21" s="30" t="s">
         <v>283</v>
       </c>
-      <c r="R21" s="31"/>
-      <c r="S21" s="31"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="30"/>
     </row>
     <row r="22" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="31" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="G22" s="31" t="s">
+      <c r="G22" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="33" t="s">
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="L22" s="31" t="s">
+      <c r="L22" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="31" t="s">
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="30" t="s">
         <v>259</v>
       </c>
-      <c r="Q22" s="31" t="s">
+      <c r="Q22" s="30" t="s">
         <v>284</v>
       </c>
-      <c r="R22" s="31"/>
-      <c r="S22" s="31"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="30"/>
     </row>
     <row r="23" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="31" t="s">
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="33" t="s">
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="L23" s="31" t="s">
+      <c r="L23" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="31" t="s">
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="30" t="s">
         <v>260</v>
       </c>
-      <c r="Q23" s="31" t="s">
+      <c r="Q23" s="30" t="s">
         <v>285</v>
       </c>
-      <c r="R23" s="31"/>
-      <c r="S23" s="31"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="30"/>
     </row>
     <row r="24" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="31" t="s">
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="31" t="s">
+      <c r="G24" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="33" t="s">
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="L24" s="31" t="s">
+      <c r="L24" s="30" t="s">
         <v>229</v>
       </c>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="31" t="s">
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="30" t="s">
         <v>261</v>
       </c>
-      <c r="Q24" s="31" t="s">
+      <c r="Q24" s="30" t="s">
         <v>286</v>
       </c>
-      <c r="R24" s="31"/>
-      <c r="S24" s="31"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
     </row>
     <row r="25" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="59" t="s">
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="60" t="s">
         <v>183</v>
       </c>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="33" t="s">
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="32" t="s">
         <v>219</v>
       </c>
-      <c r="L25" s="31" t="s">
+      <c r="L25" s="30" t="s">
         <v>230</v>
       </c>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="31" t="s">
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="30" t="s">
         <v>262</v>
       </c>
-      <c r="Q25" s="31" t="s">
+      <c r="Q25" s="30" t="s">
         <v>287</v>
       </c>
-      <c r="R25" s="31"/>
-      <c r="S25" s="31"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="30"/>
     </row>
     <row r="26" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="31" t="s">
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="G26" s="31" t="s">
+      <c r="G26" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="H26" s="31" t="s">
+      <c r="H26" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="I26" s="31" t="s">
+      <c r="I26" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="J26" s="32"/>
-      <c r="K26" s="33" t="s">
+      <c r="J26" s="31"/>
+      <c r="K26" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="L26" s="31" t="s">
+      <c r="L26" s="30" t="s">
         <v>231</v>
       </c>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="32"/>
-      <c r="P26" s="31" t="s">
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="30" t="s">
         <v>263</v>
       </c>
-      <c r="Q26" s="31" t="s">
+      <c r="Q26" s="30" t="s">
         <v>288</v>
       </c>
-      <c r="R26" s="31"/>
-      <c r="S26" s="31"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="30"/>
     </row>
     <row r="27" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="31" t="s">
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G27" s="31" t="s">
+      <c r="G27" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="33" t="s">
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="32" t="s">
         <v>221</v>
       </c>
-      <c r="L27" s="31" t="s">
+      <c r="L27" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="32"/>
-      <c r="P27" s="31" t="s">
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="Q27" s="31" t="s">
+      <c r="Q27" s="30" t="s">
         <v>289</v>
       </c>
-      <c r="R27" s="31"/>
-      <c r="S27" s="31"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="30"/>
     </row>
     <row r="28" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="31" t="s">
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G28" s="31" t="s">
+      <c r="G28" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="33" t="s">
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="L28" s="31" t="s">
+      <c r="L28" s="30" t="s">
         <v>233</v>
       </c>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="32"/>
-      <c r="P28" s="31" t="s">
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="30" t="s">
         <v>265</v>
       </c>
-      <c r="Q28" s="31" t="s">
+      <c r="Q28" s="30" t="s">
         <v>290</v>
       </c>
-      <c r="R28" s="31"/>
-      <c r="S28" s="31"/>
+      <c r="R28" s="30"/>
+      <c r="S28" s="30"/>
     </row>
     <row r="29" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="31" t="s">
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="31" t="s">
+      <c r="G29" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="33" t="s">
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="32" t="s">
         <v>223</v>
       </c>
-      <c r="L29" s="31" t="s">
+      <c r="L29" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="32"/>
-      <c r="P29" s="31" t="s">
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="30" t="s">
         <v>260</v>
       </c>
-      <c r="Q29" s="31" t="s">
+      <c r="Q29" s="30" t="s">
         <v>291</v>
       </c>
-      <c r="R29" s="31"/>
-      <c r="S29" s="31"/>
+      <c r="R29" s="30"/>
+      <c r="S29" s="30"/>
     </row>
     <row r="30" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="31" t="s">
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="31" t="s">
+      <c r="G30" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="33" t="s">
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="32" t="s">
         <v>224</v>
       </c>
-      <c r="L30" s="31" t="s">
+      <c r="L30" s="30" t="s">
         <v>235</v>
       </c>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="32"/>
-      <c r="P30" s="31" t="s">
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="31"/>
+      <c r="P30" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="Q30" s="31" t="s">
+      <c r="Q30" s="30" t="s">
         <v>292</v>
       </c>
-      <c r="R30" s="31"/>
-      <c r="S30" s="31"/>
+      <c r="R30" s="30"/>
+      <c r="S30" s="30"/>
     </row>
     <row r="31" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="31" t="s">
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G31" s="31" t="s">
+      <c r="G31" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="69" t="s">
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="58" t="s">
         <v>236</v>
       </c>
-      <c r="L31" s="70"/>
-      <c r="M31" s="70"/>
-      <c r="N31" s="70"/>
-      <c r="O31" s="32"/>
-      <c r="P31" s="31" t="s">
+      <c r="L31" s="59"/>
+      <c r="M31" s="59"/>
+      <c r="N31" s="59"/>
+      <c r="O31" s="31"/>
+      <c r="P31" s="30" t="s">
         <v>267</v>
       </c>
-      <c r="Q31" s="31" t="s">
+      <c r="Q31" s="30" t="s">
         <v>293</v>
       </c>
-      <c r="R31" s="31"/>
-      <c r="S31" s="31"/>
+      <c r="R31" s="30"/>
+      <c r="S31" s="30"/>
     </row>
     <row r="32" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="31" t="s">
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="G32" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="67" t="s">
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="L32" s="68"/>
-      <c r="M32" s="31" t="s">
+      <c r="L32" s="70"/>
+      <c r="M32" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="N32" s="31" t="s">
+      <c r="N32" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="O32" s="32"/>
-      <c r="P32" s="31"/>
-      <c r="Q32" s="31"/>
-      <c r="R32" s="31"/>
-      <c r="S32" s="31"/>
+      <c r="O32" s="31"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="30"/>
+      <c r="R32" s="30"/>
+      <c r="S32" s="30"/>
     </row>
     <row r="33" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="31" t="s">
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="31" t="s">
+      <c r="G33" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="65" t="s">
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="56" t="s">
         <v>237</v>
       </c>
-      <c r="L33" s="66"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="32"/>
-      <c r="P33" s="59" t="s">
+      <c r="L33" s="57"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="31"/>
+      <c r="P33" s="60" t="s">
         <v>242</v>
       </c>
-      <c r="Q33" s="60"/>
-      <c r="R33" s="60"/>
-      <c r="S33" s="60"/>
+      <c r="Q33" s="61"/>
+      <c r="R33" s="61"/>
+      <c r="S33" s="61"/>
     </row>
     <row r="34" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="31" t="s">
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="31" t="s">
+      <c r="G34" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="69" t="s">
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="58" t="s">
         <v>238</v>
       </c>
-      <c r="L34" s="70"/>
-      <c r="M34" s="70"/>
-      <c r="N34" s="70"/>
-      <c r="O34" s="32"/>
-      <c r="P34" s="31" t="s">
+      <c r="L34" s="59"/>
+      <c r="M34" s="59"/>
+      <c r="N34" s="59"/>
+      <c r="O34" s="31"/>
+      <c r="P34" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="Q34" s="31" t="s">
+      <c r="Q34" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="R34" s="31" t="s">
+      <c r="R34" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="S34" s="31" t="s">
+      <c r="S34" s="30" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="59" t="s">
+      <c r="A35" s="60" t="s">
         <v>154</v>
       </c>
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="31" t="s">
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="G35" s="31" t="s">
+      <c r="G35" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="67" t="s">
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="L35" s="68"/>
-      <c r="M35" s="31" t="s">
+      <c r="L35" s="70"/>
+      <c r="M35" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="N35" s="31" t="s">
+      <c r="N35" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="O35" s="34"/>
-      <c r="P35" s="31" t="s">
+      <c r="O35" s="33"/>
+      <c r="P35" s="30" t="s">
         <v>72</v>
       </c>
       <c r="Q35" s="24" t="s">
         <v>294</v>
       </c>
-      <c r="R35" s="31"/>
-      <c r="S35" s="31"/>
+      <c r="R35" s="30"/>
+      <c r="S35" s="30"/>
     </row>
     <row r="36" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="C36" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="31" t="s">
+      <c r="E36" s="31"/>
+      <c r="F36" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="G36" s="31" t="s">
+      <c r="G36" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="65" t="s">
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="56" t="s">
         <v>239</v>
       </c>
-      <c r="L36" s="66"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="31" t="s">
+      <c r="L36" s="57"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="30"/>
+      <c r="O36" s="31"/>
+      <c r="P36" s="30" t="s">
         <v>73</v>
       </c>
       <c r="Q36" s="24" t="s">
         <v>295</v>
       </c>
-      <c r="R36" s="31"/>
-      <c r="S36" s="31"/>
+      <c r="R36" s="30"/>
+      <c r="S36" s="30"/>
     </row>
     <row r="37" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="31" t="s">
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="G37" s="31" t="s">
+      <c r="G37" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="69" t="s">
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="L37" s="70"/>
-      <c r="M37" s="70"/>
-      <c r="N37" s="70"/>
-      <c r="O37" s="32"/>
-      <c r="P37" s="31" t="s">
+      <c r="L37" s="59"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="59"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="30" t="s">
         <v>74</v>
       </c>
       <c r="Q37" s="24" t="s">
         <v>296</v>
       </c>
-      <c r="R37" s="31"/>
-      <c r="S37" s="31"/>
+      <c r="R37" s="30"/>
+      <c r="S37" s="30"/>
     </row>
     <row r="38" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="31" t="s">
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="31" t="s">
+      <c r="G38" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="33" t="s">
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="L38" s="31" t="s">
+      <c r="L38" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="M38" s="31" t="s">
+      <c r="M38" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="N38" s="31" t="s">
+      <c r="N38" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="O38" s="32"/>
-      <c r="P38" s="31" t="s">
+      <c r="O38" s="31"/>
+      <c r="P38" s="30" t="s">
         <v>75</v>
       </c>
       <c r="Q38" s="24" t="s">
         <v>297</v>
       </c>
-      <c r="R38" s="31"/>
-      <c r="S38" s="31"/>
+      <c r="R38" s="30"/>
+      <c r="S38" s="30"/>
     </row>
     <row r="39" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="31" t="s">
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="G39" s="31" t="s">
+      <c r="G39" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="33"/>
-      <c r="L39" s="31"/>
-      <c r="M39" s="31"/>
-      <c r="N39" s="31"/>
-      <c r="O39" s="32"/>
-      <c r="P39" s="31" t="s">
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="32"/>
+      <c r="L39" s="30"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="30"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="30" t="s">
         <v>76</v>
       </c>
       <c r="Q39" s="24" t="s">
         <v>298</v>
       </c>
-      <c r="R39" s="31"/>
-      <c r="S39" s="31"/>
+      <c r="R39" s="30"/>
+      <c r="S39" s="30"/>
     </row>
     <row r="40" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="31" t="s">
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="G40" s="31" t="s">
+      <c r="G40" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="33"/>
-      <c r="L40" s="31"/>
-      <c r="M40" s="31"/>
-      <c r="N40" s="31"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="31" t="s">
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="32"/>
+      <c r="L40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="30" t="s">
         <v>77</v>
       </c>
       <c r="Q40" s="24" t="s">
         <v>299</v>
       </c>
-      <c r="R40" s="31"/>
-      <c r="S40" s="31"/>
+      <c r="R40" s="30"/>
+      <c r="S40" s="30"/>
     </row>
     <row r="41" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="31" t="s">
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="31" t="s">
+      <c r="G41" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="33"/>
-      <c r="L41" s="31"/>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="31" t="s">
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="30"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="30" t="s">
         <v>78</v>
       </c>
       <c r="Q41" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="R41" s="31"/>
-      <c r="S41" s="31"/>
+      <c r="R41" s="30"/>
+      <c r="S41" s="30"/>
     </row>
     <row r="42" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="31" t="s">
+      <c r="B42" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="31" t="s">
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="G42" s="31" t="s">
+      <c r="G42" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="33"/>
-      <c r="L42" s="31"/>
-      <c r="M42" s="31"/>
-      <c r="N42" s="31"/>
-      <c r="O42" s="32"/>
-      <c r="P42" s="31" t="s">
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="31"/>
+      <c r="K42" s="32"/>
+      <c r="L42" s="30"/>
+      <c r="M42" s="30"/>
+      <c r="N42" s="30"/>
+      <c r="O42" s="31"/>
+      <c r="P42" s="30" t="s">
         <v>79</v>
       </c>
       <c r="Q42" s="24" t="s">
         <v>301</v>
       </c>
-      <c r="R42" s="31"/>
-      <c r="S42" s="31"/>
+      <c r="R42" s="30"/>
+      <c r="S42" s="30"/>
     </row>
     <row r="43" spans="1:19" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="33"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="31"/>
-      <c r="N43" s="31"/>
-      <c r="O43" s="32"/>
-      <c r="P43" s="31"/>
-      <c r="Q43" s="31"/>
-      <c r="R43" s="31"/>
-      <c r="S43" s="31"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="30"/>
+      <c r="M43" s="30"/>
+      <c r="N43" s="30"/>
+      <c r="O43" s="31"/>
+      <c r="P43" s="30"/>
+      <c r="Q43" s="30"/>
+      <c r="R43" s="30"/>
+      <c r="S43" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K35:L35"/>
     <mergeCell ref="K36:L36"/>
     <mergeCell ref="K37:N37"/>
     <mergeCell ref="P4:S4"/>
@@ -3989,12 +3991,11 @@
     <mergeCell ref="K33:L33"/>
     <mergeCell ref="K32:L32"/>
     <mergeCell ref="K34:N34"/>
-    <mergeCell ref="K35:L35"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="73" orientation="landscape" horizontalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>